<commit_message>
add to cart feature
</commit_message>
<xml_diff>
--- a/api.xlsx
+++ b/api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jonathan\Desktop\shopping-online-site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEDEC8C-A87D-4B88-968F-8FBE53BAA402}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240CD612-3733-4B35-ACF7-F0BA0E618043}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{CD2936B8-A627-4958-BE58-95644BC451E9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -446,6 +446,26 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>POST
+/add_item_cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">request{
+item_id,
+amount,
+}response{
+all cart items with the cart data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">get all cart items for thet client and add it to session 
+if the cart has this item so update if not do and update session and return
+same thing with delete if it exsist in the session so update if not so delete after order is placed delet cart items and  create new cart id
+q: what happpends if somone on another site logs in and changes things around so we need to have a session saver a: what we need to do is save a session to a user on the data base on delete it on log out) </t>
   </si>
 </sst>
 </file>
@@ -844,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C0245B-8207-4550-8313-2CC12A41A84B}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,28 +1048,40 @@
       <c r="A16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>

</xml_diff>